<commit_message>
Added Insteract and PartnersGroup POC Projects
</commit_message>
<xml_diff>
--- a/Insteract.POC/test-data/TestData.xlsx
+++ b/Insteract.POC/test-data/TestData.xlsx
@@ -4,16 +4,105 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Create User" sheetId="1" r:id="rId1"/>
-    <sheet name="User" sheetId="2" r:id="rId2"/>
-    <sheet name="TR" sheetId="3" r:id="rId3"/>
-    <sheet name="Mail" sheetId="4" r:id="rId4"/>
+    <sheet name="Login" sheetId="6" r:id="rId2"/>
+    <sheet name="ResetPassword" sheetId="7" r:id="rId3"/>
+    <sheet name="SearchFlights" sheetId="8" r:id="rId4"/>
+    <sheet name="TrMail" sheetId="9" r:id="rId5"/>
+    <sheet name="Users" sheetId="10" r:id="rId6"/>
+    <sheet name="Mailinator" sheetId="11" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
+  <si>
+    <t>UniqueValue</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Demo001</t>
+  </si>
+  <si>
+    <t>INS101@mailinator.com</t>
+  </si>
+  <si>
+    <t>insteract01</t>
+  </si>
+  <si>
+    <t>INS101-2@mailinator.com</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Insteract - Password reset request</t>
+  </si>
+  <si>
+    <t>Employee ID</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>Demo002</t>
+  </si>
+  <si>
+    <t>BLR</t>
+  </si>
+  <si>
+    <t>MAA</t>
+  </si>
+  <si>
+    <t>INS101-1@mailinator.com</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Approver</t>
+  </si>
+  <si>
+    <t>INS101-1</t>
+  </si>
+  <si>
+    <t>INS101-2</t>
+  </si>
+  <si>
+    <t>INS101-Auto9-FN</t>
+  </si>
+  <si>
+    <t>INS101-Auto9-LN</t>
+  </si>
+  <si>
+    <t>INS101-Auto9@mailinator.com</t>
+  </si>
+  <si>
+    <t>IDAuto009</t>
+  </si>
+  <si>
+    <t>INS101-9@mailinator.com</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -47,8 +136,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -343,48 +433,357 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>